<commit_message>
cambio de unidad de medicion del gant de instalacion
</commit_message>
<xml_diff>
--- a/Instalacion_de_red/Gant_instalacion_v1.xlsx
+++ b/Instalacion_de_red/Gant_instalacion_v1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\cosas de tareas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d890185b7940047/Escuela/ico/octavo/Redes2/ProyectoRedes/Soporte/Instalacion_de_red/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9AC3EC7-66DE-4755-B3DA-C75583A6AB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{A9AC3EC7-66DE-4755-B3DA-C75583A6AB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C49D3519-772C-4C1E-A3E9-24DFBAE2857E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{29B149B4-ABA8-4064-B5BE-943735770EF0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{29B149B4-ABA8-4064-B5BE-943735770EF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>Configuración de ip</t>
   </si>
   <si>
-    <t>Duración(semanas)</t>
-  </si>
-  <si>
     <t>Petición y recepción del equipo</t>
   </si>
   <si>
@@ -90,13 +87,29 @@
   </si>
   <si>
     <t>Semanas</t>
+  </si>
+  <si>
+    <r>
+      <t>Duración</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(Días)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +127,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,7 +208,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -216,6 +237,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -225,8 +247,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFD7819E-EA71-4059-B3A6-C197A1E6BC72}">
   <dimension ref="A3:AB27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="U13" sqref="U13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,120 +586,120 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D3" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="15"/>
-      <c r="L3" s="15"/>
-      <c r="M3" s="15"/>
-      <c r="N3" s="15"/>
-      <c r="O3" s="15"/>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="15"/>
-      <c r="S3" s="15"/>
-      <c r="T3" s="15"/>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
-      <c r="W3" s="15"/>
-      <c r="X3" s="15"/>
-      <c r="Y3" s="15"/>
-      <c r="Z3" s="15"/>
-      <c r="AA3" s="15"/>
-      <c r="AB3" s="15"/>
+      <c r="D3" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="14"/>
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
     </row>
     <row r="4" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4">
+        <v>7</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <v>10</v>
+      </c>
+      <c r="N4">
+        <v>11</v>
+      </c>
+      <c r="O4">
         <v>12</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="14">
-        <v>1</v>
-      </c>
-      <c r="E4" s="14">
-        <v>2</v>
-      </c>
-      <c r="F4" s="14">
-        <v>3</v>
-      </c>
-      <c r="G4" s="14">
-        <v>4</v>
-      </c>
-      <c r="H4" s="14">
-        <v>5</v>
-      </c>
-      <c r="I4" s="14">
-        <v>6</v>
-      </c>
-      <c r="J4" s="14">
-        <v>7</v>
-      </c>
-      <c r="K4" s="14">
-        <v>8</v>
-      </c>
-      <c r="L4" s="14">
-        <v>9</v>
-      </c>
-      <c r="M4" s="14">
-        <v>10</v>
-      </c>
-      <c r="N4" s="14">
-        <v>11</v>
-      </c>
-      <c r="O4" s="14">
-        <v>12</v>
-      </c>
-      <c r="P4" s="14">
+      <c r="P4">
         <v>13</v>
       </c>
-      <c r="Q4" s="14">
+      <c r="Q4">
         <v>14</v>
       </c>
-      <c r="R4" s="14">
+      <c r="R4">
         <v>15</v>
       </c>
-      <c r="S4" s="14">
+      <c r="S4">
         <v>16</v>
       </c>
-      <c r="T4" s="14">
+      <c r="T4">
         <v>17</v>
       </c>
-      <c r="U4" s="14">
+      <c r="U4">
         <v>18</v>
       </c>
-      <c r="V4" s="14">
+      <c r="V4">
         <v>19</v>
       </c>
-      <c r="W4" s="14">
+      <c r="W4">
         <v>20</v>
       </c>
-      <c r="X4" s="14">
+      <c r="X4">
         <v>21</v>
       </c>
-      <c r="Y4" s="14">
+      <c r="Y4">
         <v>22</v>
       </c>
-      <c r="Z4" s="14">
+      <c r="Z4">
         <v>23</v>
       </c>
-      <c r="AA4" s="14">
+      <c r="AA4">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="10"/>
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="11"/>
     </row>
     <row r="6" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
@@ -688,8 +708,8 @@
       <c r="B6" s="7">
         <v>2</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -698,23 +718,23 @@
       <c r="B7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="13"/>
+      <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="7">
         <v>2</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="11"/>
+      <c r="A9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="12"/>
     </row>
     <row r="10" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
@@ -723,8 +743,8 @@
       <c r="B10" s="9">
         <v>2</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -733,8 +753,8 @@
       <c r="B11" s="9">
         <v>2</v>
       </c>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -743,7 +763,7 @@
       <c r="B12" s="9">
         <v>1</v>
       </c>
-      <c r="J12" s="13"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -752,9 +772,9 @@
       <c r="B13" s="9">
         <v>3</v>
       </c>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="13"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
     <row r="14" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -763,9 +783,9 @@
       <c r="B14" s="9">
         <v>3</v>
       </c>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="13"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
     </row>
     <row r="15" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
@@ -774,15 +794,15 @@
       <c r="B15" s="9">
         <v>3</v>
       </c>
-      <c r="Q15" s="13"/>
-      <c r="R15" s="13"/>
-      <c r="S15" s="13"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10"/>
     </row>
     <row r="16" spans="1:28" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="12"/>
+      <c r="A16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="13"/>
     </row>
     <row r="17" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
@@ -791,8 +811,8 @@
       <c r="B17" s="5">
         <v>2</v>
       </c>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
+      <c r="T17" s="10"/>
+      <c r="U17" s="10"/>
     </row>
     <row r="18" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
@@ -801,7 +821,7 @@
       <c r="B18" s="5">
         <v>1</v>
       </c>
-      <c r="V18" s="13"/>
+      <c r="V18" s="10"/>
     </row>
     <row r="19" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
@@ -810,8 +830,8 @@
       <c r="B19" s="5">
         <v>2</v>
       </c>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
     </row>
     <row r="20" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>